<commit_message>
dalsi drobne upravy kodu, zmerena zebra1
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Visual Studio 2017\Projects\HashSekv\HashSekv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754B65F1-13B6-4466-82B5-CE2A15F772ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0818996-9002-4F19-900C-6282760ABC9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11220" yWindow="2175" windowWidth="19875" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sekvenční řešení" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Heslo</t>
   </si>
@@ -288,17 +288,34 @@
   <si>
     <t>X</t>
   </si>
+  <si>
+    <t>Brute force GPU</t>
+  </si>
+  <si>
+    <t>128 vláken, 32 bloků, 1000 threshold</t>
+  </si>
+  <si>
+    <t>267,4 s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -341,8 +358,8 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -640,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,13 +851,25 @@
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
+    <row r="13" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>

</xml_diff>

<commit_message>
Pridan sekvencni rozsireny slovnikovy utok, podporujici pouze pridavani skupin znaku za slovo
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Visual Studio 2017\Projects\HashSekv\HashSekv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0818996-9002-4F19-900C-6282760ABC9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1CED39-AB31-42CC-B68D-D685E4394C01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11220" yWindow="2175" windowWidth="19875" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -292,10 +292,10 @@
     <t>Brute force GPU</t>
   </si>
   <si>
-    <t>128 vláken, 32 bloků, 1000 threshold</t>
-  </si>
-  <si>
     <t>267,4 s</t>
+  </si>
+  <si>
+    <t>128 vláken, 32 bloků, 1000 threshold (181MHash/s)</t>
   </si>
 </sst>
 </file>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,10 +865,10 @@
         <v>26</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Dokoncen rozsireny slovnikovy utok GPU, pridany nejake nove namerena data
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Visual Studio 2017\Projects\HashSekv\HashSekv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82B7D20-5733-42AF-B573-8A0C44BBD6D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE64EBC-6693-4561-87D4-CF47EF0AFBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>Heslo</t>
   </si>
@@ -170,9 +170,6 @@
     </r>
   </si>
   <si>
-    <t>Brute force</t>
-  </si>
-  <si>
     <t>malá písmena</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
 &gt;&gt; $j = Get-Date</t>
   </si>
   <si>
-    <t>Brute Force</t>
-  </si>
-  <si>
     <t>2670 ms</t>
   </si>
   <si>
@@ -302,6 +296,99 @@
   </si>
   <si>
     <t>6 znaků, iterativní řešení kolem 5 hodin!!</t>
+  </si>
+  <si>
+    <t>ZZZ989</t>
+  </si>
+  <si>
+    <t>$i = Get-Date
+&gt;&gt;  .\prc_gpu.exe 3 E:\Dictionary\words.txt 088b01dbb7d4773a093e4d087360af20 1 0 1 1 1 0 3 3
+&gt;&gt; $j = Get-Date
+&gt;&gt; $j - $i</t>
+  </si>
+  <si>
+    <t>Rozšířený slovníkový útok GPU</t>
+  </si>
+  <si>
+    <t>slovník cca. 500k slov pravidla pridavani za slovo cisla delky 1 a cisla delky 3</t>
+  </si>
+  <si>
+    <t>2504 ms</t>
+  </si>
+  <si>
+    <t>128 vláken 32 bloků, 1000 threshold, dictionary threshold 250</t>
+  </si>
+  <si>
+    <t>$i = Get-Date
+&gt;&gt;  .\prc_gpu.exe 0 E:\Dictionary\words.txt 088b01dbb7d4773a093e4d087360af20 1 0 1 1 1 0 3 3
+&gt;&gt; $j = Get-Date
+&gt;&gt; $j - $i</t>
+  </si>
+  <si>
+    <t>134 s</t>
+  </si>
+  <si>
+    <t>napalm5e</t>
+  </si>
+  <si>
+    <t>$i = Get-Date
+&gt;&gt;  .\prc_gpu.exe 3 E:\Dictionary\words.txt bd14a2ab2d51782968669b68b17d909f 1 4 2 2
+&gt;&gt; $j = Get-Date
+&gt;&gt; $j - $i</t>
+  </si>
+  <si>
+    <t>slovník cca. 500k slov, pravidla pridavani za slovo cisla a pismena delky 2</t>
+  </si>
+  <si>
+    <t>5354 ms</t>
+  </si>
+  <si>
+    <t>3711 ms</t>
+  </si>
+  <si>
+    <t>128 vláken 64 bloků, 1000 threshold, dictionary threshold 250; slovo je přibližně uprostřed slovníku</t>
+  </si>
+  <si>
+    <t>$i = Get-Date
+&gt;&gt;  .\prc_gpu.exe 0 E:\Dictionary\words.txt bd14a2ab2d51782968669b68b17d909f 1 4 2 2
+&gt;&gt; $j = Get-Date
+&gt;&gt; $j - $i</t>
+  </si>
+  <si>
+    <t>Rozšířený slovníkový útok CPU</t>
+  </si>
+  <si>
+    <t>271,7 s</t>
+  </si>
+  <si>
+    <t>$i = Get-Date
+&gt;&gt;  .\prc_gpu.exe 2 4 d3eb9a9233e52948740d7eb8c3062d14 5 5
+&gt;&gt; $j = Get-Date
+&gt;&gt; $j - $i</t>
+  </si>
+  <si>
+    <t>5284 ms</t>
+  </si>
+  <si>
+    <t>Brute force CPU</t>
+  </si>
+  <si>
+    <t>Brute Force CPU</t>
+  </si>
+  <si>
+    <t>$i = Get-Date
+&gt;&gt;  .\prc_gpu.exe 2 1 5d41402abc4b2a76b9719d911017c592 5 5
+&gt;&gt; $j = Get-Date
+&gt;&gt; $j - $i</t>
+  </si>
+  <si>
+    <t>425 ms</t>
+  </si>
+  <si>
+    <t>5 znaků, cca 60x zrychlení! 128 vláken 32 bloků, 1000 threshold, dictionary threshold 250</t>
+  </si>
+  <si>
+    <t>128 vláken 32 bloků, 1000 threshold, dictionary threshold 250, oproti slovníkovému útoku 3x rychlejší</t>
   </si>
 </sst>
 </file>
@@ -674,14 +761,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="70.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" customWidth="1"/>
@@ -709,7 +797,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="60" x14ac:dyDescent="0.25">
@@ -717,232 +805,312 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="G5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="F6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>9999</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="D8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>99999</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="C10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <v>9999</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>31</v>
+      <c r="G10" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>99999</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>32</v>
+      <c r="C11" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <v>99999</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="D20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
-        <v>99999</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
@@ -1017,6 +1185,9 @@
       <c r="G29" s="5"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:G20">
+    <sortCondition ref="D5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
do reportu pridano dalsi mereni
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Visual Studio 2017\Projects\HashSekv\HashSekv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE64EBC-6693-4561-87D4-CF47EF0AFBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D262E8-E9EE-483F-B13D-ECCB9C1E7F79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="19830" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sekvenční řešení" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>Heslo</t>
   </si>
@@ -277,9 +277,6 @@
     <t>3308 ms</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Brute force GPU</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
 &gt;&gt; $j-$i</t>
   </si>
   <si>
-    <t>6 znaků, iterativní řešení kolem 5 hodin!!</t>
-  </si>
-  <si>
     <t>ZZZ989</t>
   </si>
   <si>
@@ -389,6 +383,9 @@
   </si>
   <si>
     <t>128 vláken 32 bloků, 1000 threshold, dictionary threshold 250, oproti slovníkovému útoku 3x rychlejší</t>
+  </si>
+  <si>
+    <t>228 minut</t>
   </si>
 </sst>
 </file>
@@ -761,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>7</v>
@@ -828,7 +825,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>7</v>
@@ -848,17 +845,15 @@
         <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>40</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
@@ -868,7 +863,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>24</v>
@@ -888,7 +883,7 @@
         <v>30</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>24</v>
@@ -905,19 +900,19 @@
         <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="60" x14ac:dyDescent="0.25">
@@ -925,19 +920,19 @@
         <v>99999</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="75" x14ac:dyDescent="0.25">
@@ -945,115 +940,115 @@
         <v>5</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="G16" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="G17" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="75" x14ac:dyDescent="0.25">

</xml_diff>